<commit_message>
vysledky a oprava okna
</commit_message>
<xml_diff>
--- a/vysledky.xlsx
+++ b/vysledky.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3525" yWindow="0" windowWidth="21870" windowHeight="9975"/>
+    <workbookView xWindow="4704" yWindow="0" windowWidth="21876" windowHeight="9972"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
   <si>
     <t>test_count</t>
   </si>
@@ -75,6 +75,18 @@
   </si>
   <si>
     <t>15.8. 17:30</t>
+  </si>
+  <si>
+    <t>3 partition</t>
+  </si>
+  <si>
+    <t>18.8. 10:30</t>
+  </si>
+  <si>
+    <t>18.8. 10:15</t>
+  </si>
+  <si>
+    <t>18.8. 10:45</t>
   </si>
 </sst>
 </file>
@@ -228,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -243,6 +255,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -525,22 +538,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:T76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" customWidth="1"/>
     <col min="4" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J2" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
@@ -564,7 +583,9 @@
         <v>9</v>
       </c>
       <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
+      <c r="J3" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
@@ -576,12 +597,14 @@
       <c r="S3" s="2"/>
       <c r="T3" s="3"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="11"/>
       <c r="B4" s="5">
         <v>152</v>
       </c>
-      <c r="C4" s="5"/>
+      <c r="C4" s="5">
+        <v>0</v>
+      </c>
       <c r="D4" s="5">
         <v>74</v>
       </c>
@@ -597,20 +620,44 @@
       <c r="H4" s="5">
         <v>127</v>
       </c>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-      <c r="T4" s="6"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I4" s="14">
+        <v>0</v>
+      </c>
+      <c r="J4" s="14">
+        <v>222</v>
+      </c>
+      <c r="K4" s="14">
+        <v>0</v>
+      </c>
+      <c r="L4" s="14">
+        <v>0</v>
+      </c>
+      <c r="M4" s="14">
+        <v>0</v>
+      </c>
+      <c r="N4" s="14">
+        <v>0</v>
+      </c>
+      <c r="O4" s="14">
+        <v>0</v>
+      </c>
+      <c r="P4" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="14">
+        <v>0</v>
+      </c>
+      <c r="R4" s="14">
+        <v>0</v>
+      </c>
+      <c r="S4" s="14">
+        <v>0</v>
+      </c>
+      <c r="T4" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="11"/>
       <c r="B5" s="5">
         <v>122</v>
@@ -632,7 +679,9 @@
         <v>128</v>
       </c>
       <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
+      <c r="J5" s="14">
+        <v>252</v>
+      </c>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
@@ -644,7 +693,7 @@
       <c r="S5" s="5"/>
       <c r="T5" s="6"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="11"/>
       <c r="B6" s="5">
         <v>163</v>
@@ -666,7 +715,9 @@
         <v>120</v>
       </c>
       <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
+      <c r="J6" s="14">
+        <v>227</v>
+      </c>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
@@ -678,7 +729,7 @@
       <c r="S6" s="5"/>
       <c r="T6" s="6"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="11"/>
       <c r="B7" s="5">
         <v>159</v>
@@ -700,7 +751,9 @@
         <v>123</v>
       </c>
       <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
+      <c r="J7" s="14">
+        <v>222</v>
+      </c>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
@@ -712,7 +765,7 @@
       <c r="S7" s="5"/>
       <c r="T7" s="6"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="11"/>
       <c r="B8" s="5">
         <v>160</v>
@@ -734,7 +787,9 @@
         <v>116</v>
       </c>
       <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
+      <c r="J8" s="14">
+        <v>267</v>
+      </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
@@ -746,7 +801,7 @@
       <c r="S8" s="5"/>
       <c r="T8" s="6"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="11"/>
       <c r="B9" s="5">
         <v>123</v>
@@ -768,7 +823,9 @@
         <v>118</v>
       </c>
       <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
+      <c r="J9" s="14">
+        <v>236</v>
+      </c>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
@@ -780,7 +837,7 @@
       <c r="S9" s="5"/>
       <c r="T9" s="6"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="11"/>
       <c r="B10" s="5">
         <v>170</v>
@@ -802,7 +859,9 @@
         <v>124</v>
       </c>
       <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
+      <c r="J10" s="14">
+        <v>224</v>
+      </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
@@ -814,7 +873,7 @@
       <c r="S10" s="5"/>
       <c r="T10" s="6"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="11"/>
       <c r="B11" s="5">
         <v>153</v>
@@ -836,7 +895,9 @@
         <v>128</v>
       </c>
       <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
+      <c r="J11" s="14">
+        <v>263</v>
+      </c>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
@@ -848,7 +909,7 @@
       <c r="S11" s="5"/>
       <c r="T11" s="6"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
       <c r="B12" s="5">
         <v>122</v>
@@ -870,7 +931,9 @@
         <v>128</v>
       </c>
       <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
+      <c r="J12" s="14">
+        <v>275</v>
+      </c>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
@@ -882,7 +945,7 @@
       <c r="S12" s="5"/>
       <c r="T12" s="6"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
       <c r="B13" s="5">
         <v>149</v>
@@ -894,7 +957,9 @@
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
+      <c r="J13" s="14">
+        <v>260</v>
+      </c>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
@@ -906,7 +971,7 @@
       <c r="S13" s="5"/>
       <c r="T13" s="6"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="11"/>
       <c r="B14" s="5">
         <v>147</v>
@@ -930,7 +995,7 @@
       <c r="S14" s="5"/>
       <c r="T14" s="6"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="11"/>
       <c r="B15" s="5">
         <v>242</v>
@@ -954,7 +1019,7 @@
       <c r="S15" s="5"/>
       <c r="T15" s="6"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="11"/>
       <c r="B16" s="5">
         <v>259</v>
@@ -978,7 +1043,7 @@
       <c r="S16" s="5"/>
       <c r="T16" s="6"/>
     </row>
-    <row r="17" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="12"/>
       <c r="B17" s="5">
         <v>272</v>
@@ -1002,7 +1067,7 @@
       <c r="S17" s="5"/>
       <c r="T17" s="6"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>2</v>
       </c>
@@ -1010,9 +1075,12 @@
         <f>AVERAGEA(B4:B17)</f>
         <v>170.92857142857142</v>
       </c>
-      <c r="C18" s="2"/>
+      <c r="C18" s="2">
+        <f t="shared" ref="C18:T18" si="0">AVERAGEA(C4:C17)</f>
+        <v>0</v>
+      </c>
       <c r="D18" s="2">
-        <f t="shared" ref="D18:H18" si="0">AVERAGEA(D4:D17)</f>
+        <f t="shared" si="0"/>
         <v>109.44444444444444</v>
       </c>
       <c r="E18" s="2">
@@ -1031,20 +1099,56 @@
         <f t="shared" si="0"/>
         <v>123.55555555555556</v>
       </c>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
-      <c r="Q18" s="2"/>
-      <c r="R18" s="2"/>
-      <c r="S18" s="2"/>
-      <c r="T18" s="3"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J18" s="2">
+        <f t="shared" si="0"/>
+        <v>244.8</v>
+      </c>
+      <c r="K18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
         <v>3</v>
       </c>
@@ -1052,9 +1156,12 @@
         <f>MAX(B4:B17)</f>
         <v>272</v>
       </c>
-      <c r="C19" s="5"/>
+      <c r="C19" s="5">
+        <f t="shared" ref="C19:T19" si="1">MAX(C4:C17)</f>
+        <v>0</v>
+      </c>
       <c r="D19" s="5">
-        <f t="shared" ref="D19:G19" si="1">MAX(D4:D17)</f>
+        <f t="shared" si="1"/>
         <v>124</v>
       </c>
       <c r="E19" s="5">
@@ -1070,23 +1177,59 @@
         <v>267</v>
       </c>
       <c r="H19" s="5">
-        <f t="shared" ref="H19" si="2">MAX(H4:H17)</f>
+        <f t="shared" si="1"/>
         <v>128</v>
       </c>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
-      <c r="P19" s="5"/>
-      <c r="Q19" s="5"/>
-      <c r="R19" s="5"/>
-      <c r="S19" s="5"/>
-      <c r="T19" s="6"/>
-    </row>
-    <row r="20" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I19" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J19" s="5">
+        <f t="shared" si="1"/>
+        <v>275</v>
+      </c>
+      <c r="K19" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L19" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M19" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N19" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O19" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P19" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q19" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R19" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S19" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T19" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
         <v>4</v>
       </c>
@@ -1094,41 +1237,80 @@
         <f>MIN(B4:B17)</f>
         <v>122</v>
       </c>
-      <c r="C20" s="8"/>
+      <c r="C20" s="8">
+        <f t="shared" ref="C20:T20" si="2">MIN(C4:C17)</f>
+        <v>0</v>
+      </c>
       <c r="D20" s="8">
-        <f t="shared" ref="D20:G20" si="3">MIN(D4:D17)</f>
+        <f t="shared" si="2"/>
         <v>74</v>
       </c>
       <c r="E20" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>212</v>
       </c>
       <c r="F20" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>121</v>
       </c>
       <c r="G20" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>225</v>
       </c>
       <c r="H20" s="8">
-        <f t="shared" ref="H20" si="4">MIN(H4:H17)</f>
+        <f t="shared" si="2"/>
         <v>116</v>
       </c>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="8"/>
-      <c r="P20" s="8"/>
-      <c r="Q20" s="8"/>
-      <c r="R20" s="8"/>
-      <c r="S20" s="8"/>
-      <c r="T20" s="9"/>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I20" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J20" s="8">
+        <f t="shared" si="2"/>
+        <v>222</v>
+      </c>
+      <c r="K20" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L20" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M20" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N20" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O20" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P20" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q20" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R20" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S20" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T20" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -1150,7 +1332,7 @@
       <c r="S21" s="5"/>
       <c r="T21" s="5"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -1172,15 +1354,17 @@
       <c r="S22" s="5"/>
       <c r="T22" s="5"/>
     </row>
-    <row r="23" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>12</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="2"/>
+      <c r="C24" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -1199,14 +1383,16 @@
       <c r="S24" s="2"/>
       <c r="T24" s="3"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
         <v>14</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="5"/>
+      <c r="C25" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
@@ -1225,13 +1411,13 @@
       <c r="S25" s="5"/>
       <c r="T25" s="6"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" s="11"/>
       <c r="B26" s="4">
         <v>120</v>
       </c>
       <c r="C26" s="5">
-        <v>0</v>
+        <v>281</v>
       </c>
       <c r="D26" s="5">
         <v>0</v>
@@ -1285,12 +1471,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" s="11"/>
       <c r="B27" s="4">
         <v>119</v>
       </c>
-      <c r="C27" s="5"/>
+      <c r="C27" s="5">
+        <v>226</v>
+      </c>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
@@ -1309,12 +1497,14 @@
       <c r="S27" s="5"/>
       <c r="T27" s="6"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" s="11"/>
       <c r="B28" s="4">
         <v>110</v>
       </c>
-      <c r="C28" s="5"/>
+      <c r="C28" s="5">
+        <v>230</v>
+      </c>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
@@ -1333,12 +1523,14 @@
       <c r="S28" s="5"/>
       <c r="T28" s="6"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" s="11"/>
       <c r="B29" s="4">
         <v>114</v>
       </c>
-      <c r="C29" s="5"/>
+      <c r="C29" s="14">
+        <v>254</v>
+      </c>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
@@ -1357,12 +1549,14 @@
       <c r="S29" s="5"/>
       <c r="T29" s="6"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30" s="11"/>
       <c r="B30" s="4">
         <v>114</v>
       </c>
-      <c r="C30" s="5"/>
+      <c r="C30" s="14">
+        <v>254</v>
+      </c>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
@@ -1381,12 +1575,14 @@
       <c r="S30" s="5"/>
       <c r="T30" s="6"/>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31" s="11"/>
       <c r="B31" s="4">
         <v>115</v>
       </c>
-      <c r="C31" s="5"/>
+      <c r="C31" s="14">
+        <v>223</v>
+      </c>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
@@ -1405,12 +1601,14 @@
       <c r="S31" s="5"/>
       <c r="T31" s="6"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" s="11"/>
       <c r="B32" s="4">
         <v>116</v>
       </c>
-      <c r="C32" s="5"/>
+      <c r="C32" s="14">
+        <v>314</v>
+      </c>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
@@ -1429,12 +1627,14 @@
       <c r="S32" s="5"/>
       <c r="T32" s="6"/>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33" s="11"/>
       <c r="B33" s="4">
         <v>113</v>
       </c>
-      <c r="C33" s="5"/>
+      <c r="C33" s="14">
+        <v>228</v>
+      </c>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
@@ -1453,12 +1653,14 @@
       <c r="S33" s="5"/>
       <c r="T33" s="6"/>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34" s="11"/>
       <c r="B34" s="4">
         <v>112</v>
       </c>
-      <c r="C34" s="5"/>
+      <c r="C34" s="14">
+        <v>320</v>
+      </c>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
@@ -1477,12 +1679,14 @@
       <c r="S34" s="5"/>
       <c r="T34" s="6"/>
     </row>
-    <row r="35" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="11"/>
       <c r="B35" s="13">
         <v>116</v>
       </c>
-      <c r="C35" s="8"/>
+      <c r="C35" s="8">
+        <v>313</v>
+      </c>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
@@ -1501,258 +1705,260 @@
       <c r="S35" s="8"/>
       <c r="T35" s="9"/>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B36" s="1">
-        <f>AVERAGEA(B26:B35)</f>
+        <f t="shared" ref="B36:T36" si="3">AVERAGEA(B26:B35)</f>
         <v>114.9</v>
       </c>
       <c r="C36" s="1">
-        <f>AVERAGEA(C26:C35)</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>264.3</v>
       </c>
       <c r="D36" s="1">
-        <f>AVERAGEA(D26:D35)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E36" s="1">
-        <f>AVERAGEA(E26:E35)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F36" s="1">
-        <f>AVERAGEA(F26:F35)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G36" s="1">
-        <f>AVERAGEA(G26:G35)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H36" s="1">
-        <f>AVERAGEA(H26:H35)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I36" s="1">
-        <f>AVERAGEA(I26:I35)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J36" s="1">
-        <f>AVERAGEA(J26:J35)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K36" s="1">
-        <f>AVERAGEA(K26:K35)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L36" s="1">
-        <f>AVERAGEA(L26:L35)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M36" s="1">
-        <f>AVERAGEA(M26:M35)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N36" s="1">
-        <f>AVERAGEA(N26:N35)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O36" s="1">
-        <f>AVERAGEA(O26:O35)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P36" s="1">
-        <f>AVERAGEA(P26:P35)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q36" s="1">
-        <f>AVERAGEA(Q26:Q35)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R36" s="1">
-        <f>AVERAGEA(R26:R35)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S36" s="1">
-        <f>AVERAGEA(S26:S35)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="T36" s="10">
-        <f>AVERAGEA(T26:T35)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
         <v>3</v>
       </c>
       <c r="B37" s="4">
-        <f>MAX(B26:B35)</f>
+        <f t="shared" ref="B37:T37" si="4">MAX(B26:B35)</f>
         <v>120</v>
       </c>
       <c r="C37" s="4">
-        <f>MAX(C26:C35)</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>320</v>
       </c>
       <c r="D37" s="4">
-        <f>MAX(D26:D35)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E37" s="4">
-        <f>MAX(E26:E35)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F37" s="4">
-        <f>MAX(F26:F35)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G37" s="4">
-        <f>MAX(G26:G35)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H37" s="4">
-        <f>MAX(H26:H35)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I37" s="4">
-        <f>MAX(I26:I35)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J37" s="4">
-        <f>MAX(J26:J35)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K37" s="4">
-        <f>MAX(K26:K35)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L37" s="4">
-        <f>MAX(L26:L35)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M37" s="4">
-        <f>MAX(M26:M35)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N37" s="4">
-        <f>MAX(N26:N35)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O37" s="4">
-        <f>MAX(O26:O35)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P37" s="4">
-        <f>MAX(P26:P35)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q37" s="4">
-        <f>MAX(Q26:Q35)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="R37" s="4">
-        <f>MAX(R26:R35)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S37" s="4">
-        <f>MAX(S26:S35)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T37" s="11">
-        <f>MAX(T26:T35)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B38" s="7">
-        <f>MIN(B26:B35)</f>
+        <f t="shared" ref="B38:T38" si="5">MIN(B26:B35)</f>
         <v>110</v>
       </c>
       <c r="C38" s="7">
-        <f>MIN(C26:C35)</f>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>223</v>
       </c>
       <c r="D38" s="7">
-        <f>MIN(D26:D35)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E38" s="7">
-        <f>MIN(E26:E35)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F38" s="7">
-        <f>MIN(F26:F35)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G38" s="7">
-        <f>MIN(G26:G35)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H38" s="7">
-        <f>MIN(H26:H35)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I38" s="7">
-        <f>MIN(I26:I35)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J38" s="7">
-        <f>MIN(J26:J35)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K38" s="7">
-        <f>MIN(K26:K35)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L38" s="7">
-        <f>MIN(L26:L35)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M38" s="7">
-        <f>MIN(M26:M35)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N38" s="7">
-        <f>MIN(N26:N35)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O38" s="7">
-        <f>MIN(O26:O35)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P38" s="7">
-        <f>MIN(P26:P35)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q38" s="7">
-        <f>MIN(Q26:Q35)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="R38" s="7">
-        <f>MIN(R26:R35)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="S38" s="7">
-        <f>MIN(S26:S35)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="T38" s="12">
-        <f>MIN(T26:T35)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A42" s="10" t="s">
         <v>10</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C42" s="2"/>
+      <c r="C42" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
@@ -1771,14 +1977,16 @@
       <c r="S42" s="2"/>
       <c r="T42" s="3"/>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A43" s="11" t="s">
         <v>14</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C43" s="5"/>
+      <c r="C43" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
@@ -1797,13 +2005,13 @@
       <c r="S43" s="5"/>
       <c r="T43" s="6"/>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A44" s="11"/>
       <c r="B44" s="4">
         <v>128</v>
       </c>
       <c r="C44" s="5">
-        <v>0</v>
+        <v>312</v>
       </c>
       <c r="D44" s="5">
         <v>0</v>
@@ -1857,12 +2065,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A45" s="11"/>
       <c r="B45" s="4">
         <v>123</v>
       </c>
-      <c r="C45" s="5"/>
+      <c r="C45" s="5">
+        <v>232</v>
+      </c>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
@@ -1881,12 +2091,14 @@
       <c r="S45" s="5"/>
       <c r="T45" s="6"/>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A46" s="11"/>
       <c r="B46" s="4">
         <v>118</v>
       </c>
-      <c r="C46" s="5"/>
+      <c r="C46" s="5">
+        <v>218</v>
+      </c>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
@@ -1905,12 +2117,14 @@
       <c r="S46" s="5"/>
       <c r="T46" s="6"/>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A47" s="11"/>
       <c r="B47" s="4">
         <v>134</v>
       </c>
-      <c r="C47" s="5"/>
+      <c r="C47" s="14">
+        <v>312</v>
+      </c>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
@@ -1929,12 +2143,14 @@
       <c r="S47" s="5"/>
       <c r="T47" s="6"/>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A48" s="11"/>
       <c r="B48" s="4">
         <v>120</v>
       </c>
-      <c r="C48" s="5"/>
+      <c r="C48" s="14">
+        <v>214</v>
+      </c>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
@@ -1953,12 +2169,14 @@
       <c r="S48" s="5"/>
       <c r="T48" s="6"/>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A49" s="11"/>
       <c r="B49" s="4">
         <v>119</v>
       </c>
-      <c r="C49" s="5"/>
+      <c r="C49" s="14">
+        <v>220</v>
+      </c>
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
@@ -1977,12 +2195,14 @@
       <c r="S49" s="5"/>
       <c r="T49" s="6"/>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A50" s="11"/>
       <c r="B50" s="4">
         <v>119</v>
       </c>
-      <c r="C50" s="5"/>
+      <c r="C50" s="14">
+        <v>247</v>
+      </c>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
@@ -2001,12 +2221,14 @@
       <c r="S50" s="5"/>
       <c r="T50" s="6"/>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A51" s="11"/>
       <c r="B51" s="4">
         <v>119</v>
       </c>
-      <c r="C51" s="5"/>
+      <c r="C51" s="14">
+        <v>253</v>
+      </c>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
       <c r="F51" s="5"/>
@@ -2025,12 +2247,14 @@
       <c r="S51" s="5"/>
       <c r="T51" s="6"/>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A52" s="11"/>
       <c r="B52" s="4">
         <v>143</v>
       </c>
-      <c r="C52" s="5"/>
+      <c r="C52" s="14">
+        <v>251</v>
+      </c>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
       <c r="F52" s="5"/>
@@ -2049,12 +2273,14 @@
       <c r="S52" s="5"/>
       <c r="T52" s="6"/>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A53" s="11"/>
       <c r="B53" s="4">
         <v>140</v>
       </c>
-      <c r="C53" s="5"/>
+      <c r="C53" s="14">
+        <v>232</v>
+      </c>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
       <c r="F53" s="5"/>
@@ -2073,12 +2299,14 @@
       <c r="S53" s="5"/>
       <c r="T53" s="6"/>
     </row>
-    <row r="54" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="11"/>
       <c r="B54" s="7">
         <v>121</v>
       </c>
-      <c r="C54" s="8"/>
+      <c r="C54" s="8">
+        <v>311</v>
+      </c>
       <c r="D54" s="8"/>
       <c r="E54" s="8"/>
       <c r="F54" s="8"/>
@@ -2097,7 +2325,7 @@
       <c r="S54" s="8"/>
       <c r="T54" s="9"/>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A55" s="10" t="s">
         <v>2</v>
       </c>
@@ -2106,79 +2334,79 @@
         <v>125.81818181818181</v>
       </c>
       <c r="C55" s="1">
-        <f t="shared" ref="C55:T55" si="5">AVERAGEA(C44:C54)</f>
-        <v>0</v>
+        <f t="shared" ref="C55:T55" si="6">AVERAGEA(C44:C54)</f>
+        <v>254.72727272727272</v>
       </c>
       <c r="D55" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E55" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F55" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G55" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H55" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I55" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J55" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K55" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="L55" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M55" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="N55" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O55" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="P55" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Q55" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R55" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="S55" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T55" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A56" s="11" t="s">
         <v>3</v>
       </c>
@@ -2187,79 +2415,79 @@
         <v>143</v>
       </c>
       <c r="C56" s="4">
-        <f t="shared" ref="C56:T56" si="6">MAX(C44:C54)</f>
-        <v>0</v>
+        <f t="shared" ref="C56:T56" si="7">MAX(C44:C54)</f>
+        <v>312</v>
       </c>
       <c r="D56" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="E56" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F56" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G56" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H56" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="I56" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J56" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K56" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L56" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M56" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N56" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="O56" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P56" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Q56" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="R56" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="S56" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T56" s="11">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="12" t="s">
         <v>4</v>
       </c>
@@ -2268,80 +2496,80 @@
         <v>118</v>
       </c>
       <c r="C57" s="7">
-        <f t="shared" ref="C57:T57" si="7">MIN(C44:C54)</f>
-        <v>0</v>
+        <f t="shared" ref="C57:T57" si="8">MIN(C44:C54)</f>
+        <v>214</v>
       </c>
       <c r="D57" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="E57" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F57" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G57" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="H57" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I57" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J57" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K57" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L57" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="M57" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="N57" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O57" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="P57" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q57" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="R57" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="S57" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="T57" s="12">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A61" s="10" t="s">
         <v>15</v>
       </c>
@@ -2367,7 +2595,7 @@
       <c r="S61" s="2"/>
       <c r="T61" s="3"/>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A62" s="11" t="s">
         <v>14</v>
       </c>
@@ -2393,7 +2621,7 @@
       <c r="S62" s="5"/>
       <c r="T62" s="6"/>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A63" s="11"/>
       <c r="B63" s="4">
         <v>12</v>
@@ -2453,7 +2681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A64" s="11"/>
       <c r="B64" s="4"/>
       <c r="C64" s="5"/>
@@ -2475,7 +2703,7 @@
       <c r="S64" s="5"/>
       <c r="T64" s="6"/>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A65" s="11"/>
       <c r="B65" s="4"/>
       <c r="C65" s="5"/>
@@ -2497,7 +2725,7 @@
       <c r="S65" s="5"/>
       <c r="T65" s="6"/>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A66" s="11"/>
       <c r="B66" s="4"/>
       <c r="C66" s="5"/>
@@ -2519,7 +2747,7 @@
       <c r="S66" s="5"/>
       <c r="T66" s="6"/>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A67" s="11"/>
       <c r="B67" s="4"/>
       <c r="C67" s="5"/>
@@ -2541,7 +2769,7 @@
       <c r="S67" s="5"/>
       <c r="T67" s="6"/>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A68" s="11"/>
       <c r="B68" s="4"/>
       <c r="C68" s="5"/>
@@ -2563,7 +2791,7 @@
       <c r="S68" s="5"/>
       <c r="T68" s="6"/>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A69" s="11"/>
       <c r="B69" s="4"/>
       <c r="C69" s="5"/>
@@ -2585,7 +2813,7 @@
       <c r="S69" s="5"/>
       <c r="T69" s="6"/>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A70" s="11"/>
       <c r="B70" s="4"/>
       <c r="C70" s="5"/>
@@ -2607,7 +2835,7 @@
       <c r="S70" s="5"/>
       <c r="T70" s="6"/>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A71" s="11"/>
       <c r="B71" s="4"/>
       <c r="C71" s="5"/>
@@ -2629,7 +2857,7 @@
       <c r="S71" s="5"/>
       <c r="T71" s="6"/>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A72" s="11"/>
       <c r="B72" s="4"/>
       <c r="C72" s="5"/>
@@ -2651,7 +2879,7 @@
       <c r="S72" s="5"/>
       <c r="T72" s="6"/>
     </row>
-    <row r="73" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="11"/>
       <c r="B73" s="7"/>
       <c r="C73" s="8"/>
@@ -2673,7 +2901,7 @@
       <c r="S73" s="8"/>
       <c r="T73" s="9"/>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A74" s="10" t="s">
         <v>2</v>
       </c>
@@ -2682,79 +2910,79 @@
         <v>12</v>
       </c>
       <c r="C74" s="1">
-        <f t="shared" ref="C74" si="8">AVERAGEA(C63:C73)</f>
+        <f t="shared" ref="C74" si="9">AVERAGEA(C63:C73)</f>
         <v>0</v>
       </c>
       <c r="D74" s="1">
-        <f t="shared" ref="D74" si="9">AVERAGEA(D63:D73)</f>
+        <f t="shared" ref="D74" si="10">AVERAGEA(D63:D73)</f>
         <v>0</v>
       </c>
       <c r="E74" s="1">
-        <f t="shared" ref="E74" si="10">AVERAGEA(E63:E73)</f>
+        <f t="shared" ref="E74" si="11">AVERAGEA(E63:E73)</f>
         <v>0</v>
       </c>
       <c r="F74" s="1">
-        <f t="shared" ref="F74" si="11">AVERAGEA(F63:F73)</f>
+        <f t="shared" ref="F74" si="12">AVERAGEA(F63:F73)</f>
         <v>0</v>
       </c>
       <c r="G74" s="1">
-        <f t="shared" ref="G74" si="12">AVERAGEA(G63:G73)</f>
+        <f t="shared" ref="G74" si="13">AVERAGEA(G63:G73)</f>
         <v>0</v>
       </c>
       <c r="H74" s="1">
-        <f t="shared" ref="H74" si="13">AVERAGEA(H63:H73)</f>
+        <f t="shared" ref="H74" si="14">AVERAGEA(H63:H73)</f>
         <v>0</v>
       </c>
       <c r="I74" s="1">
-        <f t="shared" ref="I74" si="14">AVERAGEA(I63:I73)</f>
+        <f t="shared" ref="I74" si="15">AVERAGEA(I63:I73)</f>
         <v>0</v>
       </c>
       <c r="J74" s="1">
-        <f t="shared" ref="J74" si="15">AVERAGEA(J63:J73)</f>
+        <f t="shared" ref="J74" si="16">AVERAGEA(J63:J73)</f>
         <v>0</v>
       </c>
       <c r="K74" s="1">
-        <f t="shared" ref="K74" si="16">AVERAGEA(K63:K73)</f>
+        <f t="shared" ref="K74" si="17">AVERAGEA(K63:K73)</f>
         <v>0</v>
       </c>
       <c r="L74" s="1">
-        <f t="shared" ref="L74" si="17">AVERAGEA(L63:L73)</f>
+        <f t="shared" ref="L74" si="18">AVERAGEA(L63:L73)</f>
         <v>0</v>
       </c>
       <c r="M74" s="1">
-        <f t="shared" ref="M74" si="18">AVERAGEA(M63:M73)</f>
+        <f t="shared" ref="M74" si="19">AVERAGEA(M63:M73)</f>
         <v>0</v>
       </c>
       <c r="N74" s="1">
-        <f t="shared" ref="N74" si="19">AVERAGEA(N63:N73)</f>
+        <f t="shared" ref="N74" si="20">AVERAGEA(N63:N73)</f>
         <v>0</v>
       </c>
       <c r="O74" s="1">
-        <f t="shared" ref="O74" si="20">AVERAGEA(O63:O73)</f>
+        <f t="shared" ref="O74" si="21">AVERAGEA(O63:O73)</f>
         <v>0</v>
       </c>
       <c r="P74" s="1">
-        <f t="shared" ref="P74" si="21">AVERAGEA(P63:P73)</f>
+        <f t="shared" ref="P74" si="22">AVERAGEA(P63:P73)</f>
         <v>0</v>
       </c>
       <c r="Q74" s="1">
-        <f t="shared" ref="Q74" si="22">AVERAGEA(Q63:Q73)</f>
+        <f t="shared" ref="Q74" si="23">AVERAGEA(Q63:Q73)</f>
         <v>0</v>
       </c>
       <c r="R74" s="1">
-        <f t="shared" ref="R74" si="23">AVERAGEA(R63:R73)</f>
+        <f t="shared" ref="R74" si="24">AVERAGEA(R63:R73)</f>
         <v>0</v>
       </c>
       <c r="S74" s="1">
-        <f t="shared" ref="S74" si="24">AVERAGEA(S63:S73)</f>
+        <f t="shared" ref="S74" si="25">AVERAGEA(S63:S73)</f>
         <v>0</v>
       </c>
       <c r="T74" s="10">
-        <f t="shared" ref="T74" si="25">AVERAGEA(T63:T73)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" ref="T74" si="26">AVERAGEA(T63:T73)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A75" s="11" t="s">
         <v>3</v>
       </c>
@@ -2763,79 +2991,79 @@
         <v>12</v>
       </c>
       <c r="C75" s="4">
-        <f t="shared" ref="C75:T75" si="26">MAX(C63:C73)</f>
+        <f t="shared" ref="C75:T75" si="27">MAX(C63:C73)</f>
         <v>0</v>
       </c>
       <c r="D75" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="E75" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="F75" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="G75" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="H75" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="I75" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="J75" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="K75" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="L75" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="M75" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="N75" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="O75" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="P75" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="Q75" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="R75" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="S75" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="T75" s="11">
-        <f t="shared" si="26"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="12" t="s">
         <v>4</v>
       </c>
@@ -2844,75 +3072,75 @@
         <v>12</v>
       </c>
       <c r="C76" s="7">
-        <f t="shared" ref="C76:T76" si="27">MIN(C63:C73)</f>
+        <f t="shared" ref="C76:T76" si="28">MIN(C63:C73)</f>
         <v>0</v>
       </c>
       <c r="D76" s="7">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="E76" s="7">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="F76" s="7">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="G76" s="7">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="H76" s="7">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="I76" s="7">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="J76" s="7">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="K76" s="7">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="L76" s="7">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="M76" s="7">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="N76" s="7">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="O76" s="7">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="P76" s="7">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="Q76" s="7">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="R76" s="7">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="S76" s="7">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="T76" s="12">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>